<commit_message>
Updated working database creation Files
</commit_message>
<xml_diff>
--- a/ETL/Top_50_city_data_final.xlsx
+++ b/ETL/Top_50_city_data_final.xlsx
@@ -1,33 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_har\Class\Group_8_Final_Project\ETL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Group_8_Final_Project\ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE39CE-8096-4643-AFEE-80A6BAE5C20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C48C5F-A128-4F94-A47D-4B6909E3C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Top_50_city_data_final" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -55,6 +43,9 @@
     <t>Pop_1990</t>
   </si>
   <si>
+    <t>Pop_Growth</t>
+  </si>
+  <si>
     <t>UE_2015</t>
   </si>
   <si>
@@ -431,18 +422,12 @@
   </si>
   <si>
     <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Pop_Growth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -876,7 +861,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -919,15 +904,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -955,7 +937,6 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1281,12 +1262,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1313,73 +1292,73 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -1387,25 +1366,25 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2">
         <v>542629</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>520116</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>486699</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <v>405390</v>
       </c>
-      <c r="H2" s="3">
-        <v>1.4685603152433391</v>
+      <c r="H2">
+        <v>1.47</v>
       </c>
       <c r="I2">
         <v>5.8</v>
@@ -1423,7 +1402,7 @@
         <v>4.7</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O2">
         <v>2.9</v>
@@ -1455,16 +1434,16 @@
       <c r="X2">
         <v>840</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2">
         <v>3112</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="1">
         <v>0.27</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB2" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB2">
         <v>37350</v>
       </c>
       <c r="AC2">
@@ -1479,25 +1458,25 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3">
         <v>1608139</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>1445632</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>1321045</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
         <v>983403</v>
       </c>
-      <c r="H3" s="3">
-        <v>2.4895538930942651</v>
+      <c r="H3">
+        <v>2.4900000000000002</v>
       </c>
       <c r="I3">
         <v>5.4</v>
@@ -1515,7 +1494,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O3">
         <v>1.1000000000000001</v>
@@ -1544,19 +1523,19 @@
       <c r="W3">
         <v>3.77</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3">
         <v>1280</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3">
         <v>4005</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3" s="1">
         <v>0.32</v>
       </c>
       <c r="AA3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB3" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB3">
         <v>48065</v>
       </c>
       <c r="AC3">
@@ -1571,25 +1550,25 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1">
+        <v>31</v>
+      </c>
+      <c r="D4">
         <v>504258</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>439041</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>396375</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <v>288091</v>
       </c>
-      <c r="H4" s="3">
-        <v>2.8385999005897</v>
+      <c r="H4">
+        <v>2.84</v>
       </c>
       <c r="I4">
         <v>5.2</v>
@@ -1607,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O4">
         <v>1.1000000000000001</v>
@@ -1636,19 +1615,19 @@
       <c r="W4">
         <v>3.77</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4">
         <v>1290</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4">
         <v>4005</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4" s="1">
         <v>0.32</v>
       </c>
       <c r="AA4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB4" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB4">
         <v>48065</v>
       </c>
       <c r="AC4">
@@ -1663,25 +1642,25 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1">
+        <v>38</v>
+      </c>
+      <c r="D5">
         <v>542107</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>494665</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>427652</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <v>354202</v>
       </c>
-      <c r="H5" s="3">
-        <v>2.1507830928625626</v>
+      <c r="H5">
+        <v>2.15</v>
       </c>
       <c r="I5">
         <v>11.1</v>
@@ -1699,7 +1678,7 @@
         <v>5.7</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O5">
         <v>4.2</v>
@@ -1728,19 +1707,19 @@
       <c r="W5">
         <v>3.19</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5">
         <v>1390</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Y5">
         <v>3715</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5" s="1">
         <v>0.37</v>
       </c>
       <c r="AA5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB5" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB5">
         <v>44576</v>
       </c>
       <c r="AC5">
@@ -1755,25 +1734,25 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1">
+        <v>38</v>
+      </c>
+      <c r="D6">
         <v>403455</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>347483</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>247057</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>183959</v>
       </c>
-      <c r="H6" s="3">
-        <v>4.0048766096880906</v>
+      <c r="H6">
+        <v>4</v>
       </c>
       <c r="I6">
         <v>10.3</v>
@@ -1791,7 +1770,7 @@
         <v>7.9</v>
       </c>
       <c r="N6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O6">
         <v>1.2</v>
@@ -1820,19 +1799,19 @@
       <c r="W6">
         <v>5.72</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6">
         <v>1070</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6">
         <v>4089</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6" s="1">
         <v>0.26</v>
       </c>
       <c r="AA6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB6" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB6">
         <v>49069</v>
       </c>
       <c r="AC6">
@@ -1847,25 +1826,25 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="1">
+        <v>38</v>
+      </c>
+      <c r="D7">
         <v>1013240</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>945942</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>894943</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>782248</v>
       </c>
-      <c r="H7" s="3">
-        <v>1.3020871311197668</v>
+      <c r="H7">
+        <v>1.3</v>
       </c>
       <c r="I7">
         <v>4.5999999999999996</v>
@@ -1883,7 +1862,7 @@
         <v>2.6</v>
       </c>
       <c r="N7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O7">
         <v>4.2</v>
@@ -1912,19 +1891,19 @@
       <c r="W7">
         <v>6.38</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7">
         <v>2420</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="Y7">
         <v>9507</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="Z7" s="1">
         <v>0.25</v>
       </c>
       <c r="AA7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB7" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB7">
         <v>114080</v>
       </c>
       <c r="AC7">
@@ -1939,25 +1918,25 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="1">
+        <v>38</v>
+      </c>
+      <c r="D8">
         <v>873579</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>805235</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>776733</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>723959</v>
       </c>
-      <c r="H8" s="3">
-        <v>0.94374447312968179</v>
+      <c r="H8">
+        <v>0.94</v>
       </c>
       <c r="I8">
         <v>3.7</v>
@@ -1975,7 +1954,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="N8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O8">
         <v>2.8</v>
@@ -2004,19 +1983,19 @@
       <c r="W8">
         <v>7.12</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8">
         <v>2910</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="Y8">
         <v>8691</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="Z8" s="1">
         <v>0.33</v>
       </c>
       <c r="AA8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB8" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB8">
         <v>104291</v>
       </c>
       <c r="AC8">
@@ -2031,25 +2010,25 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="1">
+        <v>38</v>
+      </c>
+      <c r="D9">
         <v>440646</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>390724</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>399484</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>372242</v>
       </c>
-      <c r="H9" s="3">
-        <v>0.84705564333991124</v>
+      <c r="H9">
+        <v>0.85</v>
       </c>
       <c r="I9">
         <v>5.9</v>
@@ -2067,7 +2046,7 @@
         <v>3.4</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O9">
         <v>2.8</v>
@@ -2096,19 +2075,19 @@
       <c r="W9">
         <v>7.2</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9">
         <v>2070</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="Y9">
         <v>8691</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Z9" s="1">
         <v>0.24</v>
       </c>
       <c r="AA9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB9" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB9">
         <v>104291</v>
       </c>
       <c r="AC9">
@@ -2123,25 +2102,25 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1">
+        <v>38</v>
+      </c>
+      <c r="D10">
         <v>3898747</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>3792621</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>3694820</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>3485398</v>
       </c>
-      <c r="H10" s="3">
-        <v>0.56193787102325476</v>
+      <c r="H10">
+        <v>0.56000000000000005</v>
       </c>
       <c r="I10">
         <v>7</v>
@@ -2159,7 +2138,7 @@
         <v>4.5</v>
       </c>
       <c r="N10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O10">
         <v>1.2</v>
@@ -2188,19 +2167,19 @@
       <c r="W10">
         <v>6.43</v>
       </c>
-      <c r="X10" s="1">
+      <c r="X10">
         <v>2300</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="Y10">
         <v>5557</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="Z10" s="1">
         <v>0.41</v>
       </c>
       <c r="AA10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB10" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB10">
         <v>66684</v>
       </c>
       <c r="AC10">
@@ -2215,25 +2194,25 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1">
+        <v>38</v>
+      </c>
+      <c r="D11">
         <v>466742</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>462257</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>461522</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>429433</v>
       </c>
-      <c r="H11" s="3">
-        <v>0.41742333718166602</v>
+      <c r="H11">
+        <v>0.42</v>
       </c>
       <c r="I11">
         <v>7.3</v>
@@ -2251,7 +2230,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="N11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O11">
         <v>1.2</v>
@@ -2280,19 +2259,19 @@
       <c r="W11">
         <v>6.43</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11">
         <v>1740</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Y11">
         <v>5557</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="Z11" s="1">
         <v>0.31</v>
       </c>
       <c r="AA11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB11" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB11">
         <v>66684</v>
       </c>
       <c r="AC11">
@@ -2307,25 +2286,25 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="1">
+        <v>38</v>
+      </c>
+      <c r="D12">
         <v>1386932</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>1307402</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>1223400</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12">
         <v>1110549</v>
       </c>
-      <c r="H12" s="3">
-        <v>1.1173948668548483</v>
+      <c r="H12">
+        <v>1.1200000000000001</v>
       </c>
       <c r="I12">
         <v>5</v>
@@ -2343,7 +2322,7 @@
         <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O12">
         <v>2.2999999999999998</v>
@@ -2372,19 +2351,19 @@
       <c r="W12">
         <v>6.33</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12">
         <v>2280</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="Y12">
         <v>5311</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="Z12" s="1">
         <v>0.43</v>
       </c>
       <c r="AA12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB12" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB12">
         <v>63726</v>
       </c>
       <c r="AC12">
@@ -2399,25 +2378,25 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1">
+        <v>38</v>
+      </c>
+      <c r="D13">
         <v>524943</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>466488</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>407018</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>369365</v>
       </c>
-      <c r="H13" s="3">
-        <v>1.7730571450603527</v>
+      <c r="H13">
+        <v>1.77</v>
       </c>
       <c r="I13">
         <v>6.4</v>
@@ -2435,7 +2414,7 @@
         <v>3.7</v>
       </c>
       <c r="N13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O13">
         <v>1.9</v>
@@ -2464,19 +2443,19 @@
       <c r="W13">
         <v>7.75</v>
       </c>
-      <c r="X13" s="1">
+      <c r="X13">
         <v>1630</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="Y13">
         <v>4904</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="Z13" s="1">
         <v>0.33</v>
       </c>
       <c r="AA13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB13" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB13">
         <v>58843</v>
       </c>
       <c r="AC13">
@@ -2491,25 +2470,25 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="1">
+        <v>53</v>
+      </c>
+      <c r="D14">
         <v>478961</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>416427</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>360890</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>281140</v>
       </c>
-      <c r="H14" s="3">
-        <v>2.699629200470266</v>
+      <c r="H14">
+        <v>2.7</v>
       </c>
       <c r="I14">
         <v>4.5</v>
@@ -2527,7 +2506,7 @@
         <v>3.2</v>
       </c>
       <c r="N14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O14">
         <v>2.4</v>
@@ -2556,19 +2535,19 @@
       <c r="W14">
         <v>2.7</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14">
         <v>1090</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Y14">
         <v>6009</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="Z14" s="1">
         <v>0.18</v>
       </c>
       <c r="AA14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB14" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB14">
         <v>72102</v>
       </c>
       <c r="AC14">
@@ -2583,25 +2562,25 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1">
+        <v>53</v>
+      </c>
+      <c r="D15">
         <v>715522</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>600158</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>554636</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>467610</v>
       </c>
-      <c r="H15" s="3">
-        <v>2.1496681436521392</v>
+      <c r="H15">
+        <v>2.15</v>
       </c>
       <c r="I15">
         <v>3.7</v>
@@ -2619,7 +2598,7 @@
         <v>2.7</v>
       </c>
       <c r="N15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O15">
         <v>2.4</v>
@@ -2648,19 +2627,19 @@
       <c r="W15">
         <v>4.1500000000000004</v>
       </c>
-      <c r="X15" s="1">
+      <c r="X15">
         <v>1620</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="Y15">
         <v>5603</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="Z15" s="1">
         <v>0.28999999999999998</v>
       </c>
       <c r="AA15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB15" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB15">
         <v>67236</v>
       </c>
       <c r="AC15">
@@ -2675,25 +2654,25 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="1">
+        <v>57</v>
+      </c>
+      <c r="D16">
         <v>689545</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>601723</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>572059</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>606900</v>
       </c>
-      <c r="H16" s="3">
-        <v>0.64038136425623726</v>
+      <c r="H16">
+        <v>0.64</v>
       </c>
       <c r="I16">
         <v>6.9</v>
@@ -2711,7 +2690,7 @@
         <v>5.5</v>
       </c>
       <c r="N16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O16">
         <v>3.6</v>
@@ -2740,19 +2719,19 @@
       <c r="W16">
         <v>5.45</v>
       </c>
-      <c r="X16" s="1">
+      <c r="X16">
         <v>2230</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="Y16">
         <v>6199</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="Z16" s="1">
         <v>0.36</v>
       </c>
       <c r="AA16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB16" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB16">
         <v>74385</v>
       </c>
       <c r="AC16">
@@ -2767,25 +2746,25 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="1">
+        <v>60</v>
+      </c>
+      <c r="D17">
         <v>442241</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>399457</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>362470</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <v>358548</v>
       </c>
-      <c r="H17" s="3">
-        <v>1.0544830959478224</v>
+      <c r="H17">
+        <v>1.05</v>
       </c>
       <c r="I17">
         <v>5.8</v>
@@ -2803,7 +2782,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="N17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O17">
         <v>1.5</v>
@@ -2832,19 +2811,19 @@
       <c r="W17">
         <v>5.32</v>
       </c>
-      <c r="X17" s="1">
+      <c r="X17">
         <v>2500</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="Y17">
         <v>5081</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="Z17" s="1">
         <v>0.49</v>
       </c>
       <c r="AA17" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB17" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB17">
         <v>60966</v>
       </c>
       <c r="AC17">
@@ -2859,25 +2838,25 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>949611</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>821784</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>735617</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18">
         <v>635230</v>
       </c>
-      <c r="H18" s="3">
-        <v>2.0306695997525548</v>
+      <c r="H18">
+        <v>2.0299999999999998</v>
       </c>
       <c r="I18">
         <v>5.9</v>
@@ -2895,7 +2874,7 @@
         <v>3.3</v>
       </c>
       <c r="N18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O18">
         <v>1.5</v>
@@ -2924,19 +2903,19 @@
       <c r="W18">
         <v>2.94</v>
       </c>
-      <c r="X18" s="1">
+      <c r="X18">
         <v>1230</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="Y18">
         <v>4285</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="Z18" s="1">
         <v>0.28999999999999998</v>
       </c>
       <c r="AA18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB18" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB18">
         <v>51421</v>
       </c>
       <c r="AC18">
@@ -2951,25 +2930,25 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="1">
+        <v>63</v>
+      </c>
+      <c r="D19">
         <v>498715</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>420003</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>416474</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <v>394017</v>
       </c>
-      <c r="H19" s="3">
-        <v>1.1851718325999183</v>
+      <c r="H19">
+        <v>1.19</v>
       </c>
       <c r="I19">
         <v>6.5</v>
@@ -2987,7 +2966,7 @@
         <v>3.7</v>
       </c>
       <c r="N19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -3016,19 +2995,19 @@
       <c r="W19">
         <v>3.81</v>
       </c>
-      <c r="X19" s="1">
+      <c r="X19">
         <v>1700</v>
       </c>
-      <c r="Y19" s="1">
+      <c r="Y19">
         <v>4546</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="Z19" s="1">
         <v>0.37</v>
       </c>
       <c r="AA19" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB19" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB19">
         <v>54557</v>
       </c>
       <c r="AC19">
@@ -3043,25 +3022,25 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1">
+        <v>66</v>
+      </c>
+      <c r="D20">
         <v>2746388</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>2695598</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>2896016</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
         <v>2783726</v>
       </c>
-      <c r="H20" s="3">
-        <v>-6.7495832772290765E-2</v>
+      <c r="H20">
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="I20">
         <v>6.6</v>
@@ -3079,7 +3058,7 @@
         <v>4</v>
       </c>
       <c r="N20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O20">
         <v>1.7</v>
@@ -3108,19 +3087,19 @@
       <c r="W20">
         <v>3.6</v>
       </c>
-      <c r="X20" s="1">
+      <c r="X20">
         <v>1600</v>
       </c>
-      <c r="Y20" s="1">
+      <c r="Y20">
         <v>5292</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="Z20" s="1">
         <v>0.3</v>
       </c>
       <c r="AA20" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB20" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB20">
         <v>63500</v>
       </c>
       <c r="AC20">
@@ -3135,25 +3114,25 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="1">
+        <v>69</v>
+      </c>
+      <c r="D21">
         <v>887642</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <v>820445</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>781870</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21">
         <v>741952</v>
       </c>
-      <c r="H21" s="3">
-        <v>0.90044966222306844</v>
+      <c r="H21">
+        <v>0.9</v>
       </c>
       <c r="I21">
         <v>5.0999999999999996</v>
@@ -3171,7 +3150,7 @@
         <v>3.3</v>
       </c>
       <c r="N21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O21">
         <v>0.5</v>
@@ -3203,16 +3182,16 @@
       <c r="X21">
         <v>950</v>
       </c>
-      <c r="Y21" s="1">
+      <c r="Y21">
         <v>4697</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="Z21" s="1">
         <v>0.2</v>
       </c>
       <c r="AA21" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB21" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB21">
         <v>56360</v>
       </c>
       <c r="AC21">
@@ -3227,25 +3206,25 @@
         <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="1">
+        <v>72</v>
+      </c>
+      <c r="D22">
         <v>397352</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
         <v>382368</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
         <v>344284</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22">
         <v>308652</v>
       </c>
-      <c r="H22" s="3">
-        <v>1.2710505902878699</v>
+      <c r="H22">
+        <v>1.27</v>
       </c>
       <c r="I22">
         <v>4.5999999999999996</v>
@@ -3263,7 +3242,7 @@
         <v>3.4</v>
       </c>
       <c r="N22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O22">
         <v>2.1</v>
@@ -3295,16 +3274,16 @@
       <c r="X22">
         <v>650</v>
       </c>
-      <c r="Y22" s="1">
+      <c r="Y22">
         <v>4697</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="Z22" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="AA22" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB22" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB22">
         <v>56360</v>
       </c>
       <c r="AC22">
@@ -3319,25 +3298,25 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="1">
+        <v>74</v>
+      </c>
+      <c r="D23">
         <v>633045</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23">
         <v>597337</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23">
         <v>256231</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23">
         <v>269063</v>
       </c>
-      <c r="H23" s="3">
-        <v>4.3708042776028577</v>
+      <c r="H23">
+        <v>4.37</v>
       </c>
       <c r="I23">
         <v>4.8</v>
@@ -3355,7 +3334,7 @@
         <v>4</v>
       </c>
       <c r="N23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O23">
         <v>1</v>
@@ -3387,16 +3366,16 @@
       <c r="X23">
         <v>980</v>
       </c>
-      <c r="Y23" s="1">
+      <c r="Y23">
         <v>4345</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="Z23" s="1">
         <v>0.23</v>
       </c>
       <c r="AA23" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB23" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB23">
         <v>52134</v>
       </c>
       <c r="AC23">
@@ -3411,25 +3390,25 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="1">
+        <v>77</v>
+      </c>
+      <c r="D24">
         <v>585708</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <v>620961</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
         <v>651154</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24">
         <v>736014</v>
       </c>
-      <c r="H24" s="3">
-        <v>-1.1356411973032499</v>
+      <c r="H24">
+        <v>-1.1399999999999999</v>
       </c>
       <c r="I24">
         <v>7.5</v>
@@ -3447,7 +3426,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="N24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O24">
         <v>2.2999999999999998</v>
@@ -3476,19 +3455,19 @@
       <c r="W24">
         <v>1.94</v>
       </c>
-      <c r="X24" s="1">
+      <c r="X24">
         <v>1300</v>
       </c>
-      <c r="Y24" s="1">
+      <c r="Y24">
         <v>5332</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="Z24" s="1">
         <v>0.24</v>
       </c>
       <c r="AA24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB24" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB24">
         <v>63988</v>
       </c>
       <c r="AC24">
@@ -3503,25 +3482,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="1">
+        <v>79</v>
+      </c>
+      <c r="D25">
         <v>675647</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
         <v>617594</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
         <v>589141</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25">
         <v>574283</v>
       </c>
-      <c r="H25" s="3">
-        <v>0.81605393604473608</v>
+      <c r="H25">
+        <v>0.82</v>
       </c>
       <c r="I25">
         <v>4.4000000000000004</v>
@@ -3539,7 +3518,7 @@
         <v>2.6</v>
       </c>
       <c r="N25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O25">
         <v>1</v>
@@ -3568,19 +3547,19 @@
       <c r="W25">
         <v>8.24</v>
       </c>
-      <c r="X25" s="1">
+      <c r="X25">
         <v>2660</v>
       </c>
-      <c r="Y25" s="1">
+      <c r="Y25">
         <v>6792</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="Z25" s="1">
         <v>0.39</v>
       </c>
       <c r="AA25" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB25" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB25">
         <v>81498</v>
       </c>
       <c r="AC25">
@@ -3595,25 +3574,25 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="1">
+        <v>82</v>
+      </c>
+      <c r="D26">
         <v>639111</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
         <v>713777</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
         <v>951270</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26">
         <v>1027974</v>
       </c>
-      <c r="H26" s="3">
-        <v>-2.3483225165227717</v>
+      <c r="H26">
+        <v>-2.35</v>
       </c>
       <c r="I26">
         <v>11.7</v>
@@ -3631,7 +3610,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="N26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O26">
         <v>5.3</v>
@@ -3660,19 +3639,19 @@
       <c r="W26">
         <v>1.39</v>
       </c>
-      <c r="X26" s="1">
+      <c r="X26">
         <v>1120</v>
       </c>
-      <c r="Y26" s="1">
+      <c r="Y26">
         <v>4514</v>
       </c>
-      <c r="Z26" s="2">
+      <c r="Z26" s="1">
         <v>0.25</v>
       </c>
       <c r="AA26" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB26" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB26">
         <v>54172</v>
       </c>
       <c r="AC26">
@@ -3687,25 +3666,25 @@
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="1">
+        <v>85</v>
+      </c>
+      <c r="D27">
         <v>429954</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27">
         <v>382578</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
         <v>382618</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27">
         <v>368383</v>
       </c>
-      <c r="H27" s="3">
-        <v>0.77576895697670789</v>
+      <c r="H27">
+        <v>0.78</v>
       </c>
       <c r="I27">
         <v>3.4</v>
@@ -3723,7 +3702,7 @@
         <v>2.8</v>
       </c>
       <c r="N27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O27">
         <v>1.2</v>
@@ -3752,19 +3731,19 @@
       <c r="W27">
         <v>3.78</v>
       </c>
-      <c r="X27" s="1">
+      <c r="X27">
         <v>1200</v>
       </c>
-      <c r="Y27" s="1">
+      <c r="Y27">
         <v>5352</v>
       </c>
-      <c r="Z27" s="2">
+      <c r="Z27" s="1">
         <v>0.22</v>
       </c>
       <c r="AA27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB27" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB27">
         <v>64225</v>
       </c>
       <c r="AC27">
@@ -3779,25 +3758,25 @@
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="1">
+        <v>88</v>
+      </c>
+      <c r="D28">
         <v>508090</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28">
         <v>459787</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
         <v>441545</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28">
         <v>435146</v>
       </c>
-      <c r="H28" s="3">
-        <v>0.77789495450444335</v>
+      <c r="H28">
+        <v>0.78</v>
       </c>
       <c r="I28">
         <v>5.7</v>
@@ -3815,7 +3794,7 @@
         <v>3.6</v>
       </c>
       <c r="N28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O28">
         <v>2.1</v>
@@ -3847,16 +3826,16 @@
       <c r="X28">
         <v>980</v>
       </c>
-      <c r="Y28" s="1">
+      <c r="Y28">
         <v>4584</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="Z28" s="1">
         <v>0.21</v>
       </c>
       <c r="AA28" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB28" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB28">
         <v>55009</v>
       </c>
       <c r="AC28">
@@ -3871,25 +3850,25 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="1">
+        <v>90</v>
+      </c>
+      <c r="D29">
         <v>486051</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <v>408958</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
         <v>409868</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29">
         <v>357807</v>
       </c>
-      <c r="H29" s="3">
-        <v>1.5433881983559994</v>
+      <c r="H29">
+        <v>1.54</v>
       </c>
       <c r="I29">
         <v>3.2</v>
@@ -3907,7 +3886,7 @@
         <v>3.3</v>
       </c>
       <c r="N29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O29">
         <v>2.2000000000000002</v>
@@ -3939,16 +3918,16 @@
       <c r="X29">
         <v>900</v>
       </c>
-      <c r="Y29" s="1">
+      <c r="Y29">
         <v>4584</v>
       </c>
-      <c r="Z29" s="2">
+      <c r="Z29" s="1">
         <v>0.2</v>
       </c>
       <c r="AA29" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB29" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB29">
         <v>55009</v>
       </c>
       <c r="AC29">
@@ -3963,25 +3942,25 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="1">
+        <v>93</v>
+      </c>
+      <c r="D30">
         <v>641903</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30">
         <v>583756</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30">
         <v>478434</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30">
         <v>258295</v>
       </c>
-      <c r="H30" s="3">
-        <v>4.656852713030335</v>
+      <c r="H30">
+        <v>4.66</v>
       </c>
       <c r="I30">
         <v>7</v>
@@ -3999,7 +3978,7 @@
         <v>4.2</v>
       </c>
       <c r="N30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O30">
         <v>18</v>
@@ -4028,19 +4007,19 @@
       <c r="W30">
         <v>3.47</v>
       </c>
-      <c r="X30" s="1">
+      <c r="X30">
         <v>1270</v>
       </c>
-      <c r="Y30" s="1">
+      <c r="Y30">
         <v>4067</v>
       </c>
-      <c r="Z30" s="2">
+      <c r="Z30" s="1">
         <v>0.31</v>
       </c>
       <c r="AA30" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB30" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB30">
         <v>48806</v>
       </c>
       <c r="AC30">
@@ -4055,25 +4034,25 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="1">
+        <v>96</v>
+      </c>
+      <c r="D31">
         <v>564559</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31">
         <v>545852</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31">
         <v>448607</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31">
         <v>384736</v>
       </c>
-      <c r="H31" s="3">
-        <v>1.9359384453878858</v>
+      <c r="H31">
+        <v>1.94</v>
       </c>
       <c r="I31">
         <v>5.8</v>
@@ -4091,7 +4070,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O31">
         <v>5.2</v>
@@ -4123,16 +4102,16 @@
       <c r="X31">
         <v>860</v>
       </c>
-      <c r="Y31" s="1">
+      <c r="Y31">
         <v>4373</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="Z31" s="1">
         <v>0.2</v>
       </c>
       <c r="AA31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB31" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB31">
         <v>52477</v>
       </c>
       <c r="AC31">
@@ -4147,25 +4126,25 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="1">
+        <v>97</v>
+      </c>
+      <c r="D32">
         <v>8804190</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32">
         <v>8175133</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32">
         <v>8008278</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32">
         <v>7322564</v>
       </c>
-      <c r="H32" s="3">
-        <v>0.92559338849889095</v>
+      <c r="H32">
+        <v>0.93</v>
       </c>
       <c r="I32">
         <v>5.7</v>
@@ -4183,7 +4162,7 @@
         <v>4</v>
       </c>
       <c r="N32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O32">
         <v>2.5</v>
@@ -4212,19 +4191,19 @@
       <c r="W32">
         <v>9.94</v>
       </c>
-      <c r="X32" s="1">
+      <c r="X32">
         <v>3260</v>
       </c>
-      <c r="Y32" s="1">
+      <c r="Y32">
         <v>6654</v>
       </c>
-      <c r="Z32" s="2">
+      <c r="Z32" s="1">
         <v>0.49</v>
       </c>
       <c r="AA32" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB32" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB32">
         <v>79844</v>
       </c>
       <c r="AC32">
@@ -4239,25 +4218,25 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="D33">
         <v>467665</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33">
         <v>403892</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33">
         <v>276093</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33">
         <v>207951</v>
       </c>
-      <c r="H33" s="3">
-        <v>4.1354727039562666</v>
+      <c r="H33">
+        <v>4.1399999999999997</v>
       </c>
       <c r="I33">
         <v>4.5999999999999996</v>
@@ -4275,7 +4254,7 @@
         <v>3.6</v>
       </c>
       <c r="N33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O33">
         <v>2.1</v>
@@ -4304,19 +4283,19 @@
       <c r="W33">
         <v>3.05</v>
       </c>
-      <c r="X33" s="1">
+      <c r="X33">
         <v>1190</v>
       </c>
-      <c r="Y33" s="1">
+      <c r="Y33">
         <v>4821</v>
       </c>
-      <c r="Z33" s="2">
+      <c r="Z33" s="1">
         <v>0.25</v>
       </c>
       <c r="AA33" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB33" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB33">
         <v>57851</v>
       </c>
       <c r="AC33">
@@ -4331,25 +4310,25 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
         <v>100</v>
       </c>
-      <c r="C34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>874579</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34">
         <v>731424</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34">
         <v>540828</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34">
         <v>395934</v>
       </c>
-      <c r="H34" s="3">
-        <v>4.0420288266731719</v>
+      <c r="H34">
+        <v>4.04</v>
       </c>
       <c r="I34">
         <v>4.9000000000000004</v>
@@ -4367,7 +4346,7 @@
         <v>3.7</v>
       </c>
       <c r="N34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O34">
         <v>4.0999999999999996</v>
@@ -4396,19 +4375,19 @@
       <c r="W34">
         <v>2.5099999999999998</v>
       </c>
-      <c r="X34" s="1">
+      <c r="X34">
         <v>1380</v>
       </c>
-      <c r="Y34" s="1">
+      <c r="Y34">
         <v>4493</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="Z34" s="1">
         <v>0.31</v>
       </c>
       <c r="AA34" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB34" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB34">
         <v>53916</v>
       </c>
       <c r="AC34">
@@ -4423,25 +4402,25 @@
         <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="1">
+        <v>104</v>
+      </c>
+      <c r="D35">
         <v>905748</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35">
         <v>787033</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35">
         <v>711470</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35">
         <v>632910</v>
       </c>
-      <c r="H35" s="3">
-        <v>1.8083200831762847</v>
+      <c r="H35">
+        <v>1.81</v>
       </c>
       <c r="I35">
         <v>4.0999999999999996</v>
@@ -4459,7 +4438,7 @@
         <v>3.6</v>
       </c>
       <c r="N35" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O35">
         <v>2.6</v>
@@ -4491,16 +4470,16 @@
       <c r="X35">
         <v>900</v>
       </c>
-      <c r="Y35" s="1">
+      <c r="Y35">
         <v>4373</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="Z35" s="1">
         <v>0.21</v>
       </c>
       <c r="AA35" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB35" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB35">
         <v>52477</v>
       </c>
       <c r="AC35">
@@ -4515,25 +4494,25 @@
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="1">
+        <v>107</v>
+      </c>
+      <c r="D36">
         <v>413066</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36">
         <v>391906</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36">
         <v>393049</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36">
         <v>367302</v>
       </c>
-      <c r="H36" s="3">
-        <v>0.58884184043916932</v>
+      <c r="H36">
+        <v>0.59</v>
       </c>
       <c r="I36">
         <v>4</v>
@@ -4551,7 +4530,7 @@
         <v>3.4</v>
       </c>
       <c r="N36" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O36">
         <v>0.8</v>
@@ -4583,16 +4562,16 @@
       <c r="X36">
         <v>880</v>
       </c>
-      <c r="Y36" s="1">
+      <c r="Y36">
         <v>4373</v>
       </c>
-      <c r="Z36" s="2">
+      <c r="Z36" s="1">
         <v>0.2</v>
       </c>
       <c r="AA36" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB36" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB36">
         <v>52477</v>
       </c>
       <c r="AC36">
@@ -4607,25 +4586,25 @@
         <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="1">
+        <v>107</v>
+      </c>
+      <c r="D37">
         <v>681054</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37">
         <v>579999</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37">
         <v>506132</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37">
         <v>444719</v>
       </c>
-      <c r="H37" s="3">
-        <v>2.1538627251839415</v>
+      <c r="H37">
+        <v>2.15</v>
       </c>
       <c r="I37">
         <v>3.7</v>
@@ -4643,7 +4622,7 @@
         <v>3.1</v>
       </c>
       <c r="N37" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O37">
         <v>1.7</v>
@@ -4675,16 +4654,16 @@
       <c r="X37">
         <v>830</v>
       </c>
-      <c r="Y37" s="1">
+      <c r="Y37">
         <v>4072</v>
       </c>
-      <c r="Z37" s="2">
+      <c r="Z37" s="1">
         <v>0.2</v>
       </c>
       <c r="AA37" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB37" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB37">
         <v>48860</v>
       </c>
       <c r="AC37">
@@ -4699,25 +4678,25 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="1">
+        <v>111</v>
+      </c>
+      <c r="D38">
         <v>652503</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38">
         <v>583776</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38">
         <v>529121</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38">
         <v>437319</v>
       </c>
-      <c r="H38" s="3">
-        <v>2.0209135975012726</v>
+      <c r="H38">
+        <v>2.02</v>
       </c>
       <c r="I38">
         <v>4.7</v>
@@ -4735,7 +4714,7 @@
         <v>3.2</v>
       </c>
       <c r="N38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="O38">
         <v>2.5</v>
@@ -4764,19 +4743,19 @@
       <c r="W38">
         <v>4.55</v>
       </c>
-      <c r="X38" s="1">
+      <c r="X38">
         <v>1490</v>
       </c>
-      <c r="Y38" s="1">
+      <c r="Y38">
         <v>4993</v>
       </c>
-      <c r="Z38" s="2">
+      <c r="Z38" s="1">
         <v>0.3</v>
       </c>
       <c r="AA38" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB38" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB38">
         <v>59921</v>
       </c>
       <c r="AC38">
@@ -4791,25 +4770,25 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="1">
+        <v>114</v>
+      </c>
+      <c r="D39">
         <v>1603797</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39">
         <v>1526006</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39">
         <v>1517550</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39">
         <v>1585577</v>
       </c>
-      <c r="H39" s="3">
-        <v>5.7144140512521702E-2</v>
+      <c r="H39">
+        <v>0.06</v>
       </c>
       <c r="I39">
         <v>7.1</v>
@@ -4827,7 +4806,7 @@
         <v>5.6</v>
       </c>
       <c r="N39" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O39">
         <v>0.9</v>
@@ -4856,19 +4835,19 @@
       <c r="W39">
         <v>3.96</v>
       </c>
-      <c r="X39" s="1">
+      <c r="X39">
         <v>1410</v>
       </c>
-      <c r="Y39" s="1">
+      <c r="Y39">
         <v>5550</v>
       </c>
-      <c r="Z39" s="2">
+      <c r="Z39" s="1">
         <v>0.25</v>
       </c>
       <c r="AA39" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB39" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB39">
         <v>66596</v>
       </c>
       <c r="AC39">
@@ -4883,25 +4862,25 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="1">
+        <v>116</v>
+      </c>
+      <c r="D40">
         <v>689447</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40">
         <v>601222</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40">
         <v>545524</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40">
         <v>510784</v>
       </c>
-      <c r="H40" s="3">
-        <v>1.5110172904313934</v>
+      <c r="H40">
+        <v>1.51</v>
       </c>
       <c r="I40">
         <v>4.4000000000000004</v>
@@ -4919,7 +4898,7 @@
         <v>2.5</v>
       </c>
       <c r="N40" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O40">
         <v>1.5</v>
@@ -4948,19 +4927,19 @@
       <c r="W40">
         <v>3.65</v>
       </c>
-      <c r="X40" s="1">
+      <c r="X40">
         <v>1640</v>
       </c>
-      <c r="Y40" s="1">
+      <c r="Y40">
         <v>5057</v>
       </c>
-      <c r="Z40" s="2">
+      <c r="Z40" s="1">
         <v>0.32</v>
       </c>
       <c r="AA40" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB40" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB40">
         <v>60680</v>
       </c>
       <c r="AC40">
@@ -4975,25 +4954,25 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41" s="1">
+        <v>116</v>
+      </c>
+      <c r="D41">
         <v>633104</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41">
         <v>646889</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41">
         <v>650100</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41">
         <v>610337</v>
       </c>
-      <c r="H41" s="3">
-        <v>0.18328497201216543</v>
+      <c r="H41">
+        <v>0.18</v>
       </c>
       <c r="I41">
         <v>7.1</v>
@@ -5011,7 +4990,7 @@
         <v>4.5</v>
       </c>
       <c r="N41" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O41">
         <v>2.2999999999999998</v>
@@ -5043,16 +5022,16 @@
       <c r="X41">
         <v>900</v>
       </c>
-      <c r="Y41" s="1">
+      <c r="Y41">
         <v>3999</v>
       </c>
-      <c r="Z41" s="2">
+      <c r="Z41" s="1">
         <v>0.23</v>
       </c>
       <c r="AA41" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB41" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB41">
         <v>47985</v>
       </c>
       <c r="AC41">
@@ -5067,25 +5046,25 @@
         <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
-      </c>
-      <c r="D42" s="1">
+        <v>120</v>
+      </c>
+      <c r="D42">
         <v>678815</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42">
         <v>649121</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42">
         <v>563662</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42">
         <v>515342</v>
       </c>
-      <c r="H42" s="3">
-        <v>1.3871218498483939</v>
+      <c r="H42">
+        <v>1.39</v>
       </c>
       <c r="I42">
         <v>4.7</v>
@@ -5103,7 +5082,7 @@
         <v>3.7</v>
       </c>
       <c r="N42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O42">
         <v>2.9</v>
@@ -5135,16 +5114,16 @@
       <c r="X42">
         <v>810</v>
       </c>
-      <c r="Y42" s="1">
+      <c r="Y42">
         <v>2709</v>
       </c>
-      <c r="Z42" s="2">
+      <c r="Z42" s="1">
         <v>0.3</v>
       </c>
       <c r="AA42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB42" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB42">
         <v>32510</v>
       </c>
       <c r="AC42">
@@ -5159,25 +5138,25 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" t="s">
         <v>120</v>
       </c>
-      <c r="C43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="1">
+      <c r="D43">
         <v>961855</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43">
         <v>790390</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43">
         <v>656562</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43">
         <v>465622</v>
       </c>
-      <c r="H43" s="3">
-        <v>3.6940425052675474</v>
+      <c r="H43">
+        <v>3.69</v>
       </c>
       <c r="I43">
         <v>3</v>
@@ -5195,7 +5174,7 @@
         <v>2.5</v>
       </c>
       <c r="N43" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O43">
         <v>2.7</v>
@@ -5224,19 +5203,19 @@
       <c r="W43">
         <v>3.53</v>
       </c>
-      <c r="X43" s="1">
+      <c r="X43">
         <v>1570</v>
       </c>
-      <c r="Y43" s="1">
+      <c r="Y43">
         <v>5165</v>
       </c>
-      <c r="Z43" s="2">
+      <c r="Z43" s="1">
         <v>0.3</v>
       </c>
       <c r="AA43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB43" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB43">
         <v>61977</v>
       </c>
       <c r="AC43">
@@ -5251,25 +5230,25 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="1">
+        <v>120</v>
+      </c>
+      <c r="D44">
         <v>2304580</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44">
         <v>2100263</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44">
         <v>1953631</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44">
         <v>1630553</v>
       </c>
-      <c r="H44" s="3">
-        <v>1.7449454881870885</v>
+      <c r="H44">
+        <v>1.74</v>
       </c>
       <c r="I44">
         <v>4.3</v>
@@ -5287,7 +5266,7 @@
         <v>3.7</v>
       </c>
       <c r="N44" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O44">
         <v>1.2</v>
@@ -5316,19 +5295,19 @@
       <c r="W44">
         <v>2.04</v>
       </c>
-      <c r="X44" s="1">
+      <c r="X44">
         <v>1210</v>
       </c>
-      <c r="Y44" s="1">
+      <c r="Y44">
         <v>4908</v>
       </c>
-      <c r="Z44" s="2">
+      <c r="Z44" s="1">
         <v>0.25</v>
       </c>
       <c r="AA44" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB44" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB44">
         <v>58890</v>
       </c>
       <c r="AC44">
@@ -5343,25 +5322,25 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="1">
+        <v>120</v>
+      </c>
+      <c r="D45">
         <v>1304379</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45">
         <v>1197816</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45">
         <v>1188580</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45">
         <v>1006877</v>
       </c>
-      <c r="H45" s="3">
-        <v>1.3027812237299763</v>
+      <c r="H45">
+        <v>1.3</v>
       </c>
       <c r="I45">
         <v>4.0999999999999996</v>
@@ -5379,7 +5358,7 @@
         <v>3.4</v>
       </c>
       <c r="N45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O45">
         <v>1.3</v>
@@ -5408,19 +5387,19 @@
       <c r="W45">
         <v>2.12</v>
       </c>
-      <c r="X45" s="1">
+      <c r="X45">
         <v>1410</v>
       </c>
-      <c r="Y45" s="1">
+      <c r="Y45">
         <v>4894</v>
       </c>
-      <c r="Z45" s="2">
+      <c r="Z45" s="1">
         <v>0.28999999999999998</v>
       </c>
       <c r="AA45" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB45" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB45">
         <v>58725</v>
       </c>
       <c r="AC45">
@@ -5435,25 +5414,25 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
-      </c>
-      <c r="D46" s="1">
+        <v>120</v>
+      </c>
+      <c r="D46">
         <v>918915</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46">
         <v>741206</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46">
         <v>534694</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46">
         <v>447619</v>
       </c>
-      <c r="H46" s="3">
-        <v>3.6617034930782388</v>
+      <c r="H46">
+        <v>3.66</v>
       </c>
       <c r="I46">
         <v>4.0999999999999996</v>
@@ -5471,7 +5450,7 @@
         <v>3.4</v>
       </c>
       <c r="N46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O46">
         <v>1.3</v>
@@ -5500,19 +5479,19 @@
       <c r="W46">
         <v>3.87</v>
       </c>
-      <c r="X46" s="1">
+      <c r="X46">
         <v>1220</v>
       </c>
-      <c r="Y46" s="1">
+      <c r="Y46">
         <v>4894</v>
       </c>
-      <c r="Z46" s="2">
+      <c r="Z46" s="1">
         <v>0.25</v>
       </c>
       <c r="AA46" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB46" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB46">
         <v>58725</v>
       </c>
       <c r="AC46">
@@ -5527,25 +5506,25 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="1">
+        <v>120</v>
+      </c>
+      <c r="D47">
         <v>394266</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47">
         <v>365438</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47">
         <v>332969</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47">
         <v>261721</v>
       </c>
-      <c r="H47" s="3">
-        <v>2.0698643949304207</v>
+      <c r="H47">
+        <v>2.0699999999999998</v>
       </c>
       <c r="I47">
         <v>4</v>
@@ -5563,7 +5542,7 @@
         <v>3.4</v>
       </c>
       <c r="N47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O47">
         <v>1.3</v>
@@ -5592,19 +5571,19 @@
       <c r="W47">
         <v>2.12</v>
       </c>
-      <c r="X47" s="1">
+      <c r="X47">
         <v>1030</v>
       </c>
-      <c r="Y47" s="1">
+      <c r="Y47">
         <v>4894</v>
       </c>
-      <c r="Z47" s="2">
+      <c r="Z47" s="1">
         <v>0.21</v>
       </c>
       <c r="AA47" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB47" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB47">
         <v>58725</v>
       </c>
       <c r="AC47">
@@ -5619,25 +5598,25 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="1">
+        <v>120</v>
+      </c>
+      <c r="D48">
         <v>1434625</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48">
         <v>1327407</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48">
         <v>1144646</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48">
         <v>935933</v>
       </c>
-      <c r="H48" s="3">
-        <v>2.1585409743652306</v>
+      <c r="H48">
+        <v>2.16</v>
       </c>
       <c r="I48">
         <v>3.7</v>
@@ -5655,7 +5634,7 @@
         <v>3.1</v>
       </c>
       <c r="N48" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O48">
         <v>3</v>
@@ -5684,19 +5663,19 @@
       <c r="W48">
         <v>2.1</v>
       </c>
-      <c r="X48" s="1">
+      <c r="X48">
         <v>1060</v>
       </c>
-      <c r="Y48" s="1">
+      <c r="Y48">
         <v>4058</v>
       </c>
-      <c r="Z48" s="2">
+      <c r="Z48" s="1">
         <v>0.26</v>
       </c>
       <c r="AA48" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB48" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB48">
         <v>48694</v>
       </c>
       <c r="AC48">
@@ -5711,25 +5690,25 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
-      </c>
-      <c r="D49" s="1">
+        <v>130</v>
+      </c>
+      <c r="D49">
         <v>459470</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49">
         <v>437994</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49">
         <v>425257</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49">
         <v>393069</v>
       </c>
-      <c r="H49" s="3">
-        <v>0.78349580158822985</v>
+      <c r="H49">
+        <v>0.78</v>
       </c>
       <c r="I49">
         <v>4.3</v>
@@ -5747,7 +5726,7 @@
         <v>2.7</v>
       </c>
       <c r="N49" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O49">
         <v>4.8</v>
@@ -5776,19 +5755,19 @@
       <c r="W49">
         <v>4.1500000000000004</v>
       </c>
-      <c r="X49" s="1">
+      <c r="X49">
         <v>1300</v>
       </c>
-      <c r="Y49" s="1">
+      <c r="Y49">
         <v>4334</v>
       </c>
-      <c r="Z49" s="2">
+      <c r="Z49" s="1">
         <v>0.3</v>
       </c>
       <c r="AA49" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB49" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB49">
         <v>52011</v>
       </c>
       <c r="AC49">
@@ -5803,25 +5782,25 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="1">
+        <v>56</v>
+      </c>
+      <c r="D50">
         <v>737015</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50">
         <v>608660</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50">
         <v>563374</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50">
         <v>516259</v>
       </c>
-      <c r="H50" s="3">
-        <v>1.7959347218920119</v>
+      <c r="H50">
+        <v>1.8</v>
       </c>
       <c r="I50">
         <v>3.8</v>
@@ -5839,7 +5818,7 @@
         <v>2.5</v>
       </c>
       <c r="N50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O50">
         <v>4</v>
@@ -5868,19 +5847,19 @@
       <c r="W50">
         <v>4.5199999999999996</v>
       </c>
-      <c r="X50" s="1">
+      <c r="X50">
         <v>1820</v>
       </c>
-      <c r="Y50" s="1">
+      <c r="Y50">
         <v>6506</v>
       </c>
-      <c r="Z50" s="2">
+      <c r="Z50" s="1">
         <v>0.28000000000000003</v>
       </c>
       <c r="AA50" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB50" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB50">
         <v>78073</v>
       </c>
       <c r="AC50">
@@ -5895,25 +5874,25 @@
         <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
-      </c>
-      <c r="D51" s="1">
+        <v>133</v>
+      </c>
+      <c r="D51">
         <v>577222</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51">
         <v>594833</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51">
         <v>596974</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51">
         <v>628088</v>
       </c>
-      <c r="H51" s="3">
-        <v>-0.42137642182920043</v>
+      <c r="H51">
+        <v>-0.42</v>
       </c>
       <c r="I51">
         <v>6.6</v>
@@ -5931,7 +5910,7 @@
         <v>4.5</v>
       </c>
       <c r="N51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O51">
         <v>2.5</v>
@@ -5963,16 +5942,16 @@
       <c r="X51">
         <v>950</v>
       </c>
-      <c r="Y51" s="1">
+      <c r="Y51">
         <v>4871</v>
       </c>
-      <c r="Z51" s="2">
+      <c r="Z51" s="1">
         <v>0.2</v>
       </c>
       <c r="AA51" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB51" s="1">
+        <v>45</v>
+      </c>
+      <c r="AB51">
         <v>58457</v>
       </c>
       <c r="AC51">

</xml_diff>